<commit_message>
Revert "Merge branch 'master' of https://github.com/king-of-kong/Machine-Learning-Nose-Jobs"
This reverts commit 3e44a7f338548100d11ada4ab811ddd218c89c3f, reversing
changes made to 7b6ad5b9cf9b2f48d77bcadaff3d9fab5122eef9.
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\GitHub\Machine-Learing-Nose-Jobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF9B6DF-857C-4CF9-A5CD-E930C3C460D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B167CAA-69DE-466A-850C-D469425622B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="1500" windowWidth="8850" windowHeight="8685" xr2:uid="{07F54489-4804-49A9-8FEB-27A3E3B3944A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{07F54489-4804-49A9-8FEB-27A3E3B3944A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -89,6 +89,9 @@
     <t>Match faces from library to XML files (the 30-40 chosen), in order to use machine learning algorithm</t>
   </si>
   <si>
+    <t>Apply changes on image of patient face for the use of the surgeon</t>
+  </si>
+  <si>
     <t>Calculate changes from the user's selected face</t>
   </si>
   <si>
@@ -98,7 +101,7 @@
     <t>Get ID 4-6 on the python app</t>
   </si>
   <si>
-    <t>Get ID 7-8 on the python app</t>
+    <t>Get ID 7-9 on the python app</t>
   </si>
 </sst>
 </file>
@@ -457,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE00F426-ABEC-4D5E-BB66-181DA25598A2}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="87.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
@@ -525,7 +528,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A13" si="0">A3 +1</f>
+        <f t="shared" ref="A4:A14" si="0">A3 +1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -619,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -637,13 +640,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -661,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -679,35 +682,53 @@
         <v>8</v>
       </c>
       <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/king-of-kong/Machine-Learning-Nose-Jobs""
This reverts commit e42111db7d79b97814bafea4dad00c5139b6aebe.
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\GitHub\Machine-Learing-Nose-Jobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B167CAA-69DE-466A-850C-D469425622B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF9B6DF-857C-4CF9-A5CD-E930C3C460D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{07F54489-4804-49A9-8FEB-27A3E3B3944A}"/>
+    <workbookView xWindow="5640" yWindow="1500" windowWidth="8850" windowHeight="8685" xr2:uid="{07F54489-4804-49A9-8FEB-27A3E3B3944A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Match faces from library to XML files (the 30-40 chosen), in order to use machine learning algorithm</t>
   </si>
   <si>
-    <t>Apply changes on image of patient face for the use of the surgeon</t>
-  </si>
-  <si>
     <t>Calculate changes from the user's selected face</t>
   </si>
   <si>
@@ -101,7 +98,7 @@
     <t>Get ID 4-6 on the python app</t>
   </si>
   <si>
-    <t>Get ID 7-9 on the python app</t>
+    <t>Get ID 7-8 on the python app</t>
   </si>
 </sst>
 </file>
@@ -460,15 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE00F426-ABEC-4D5E-BB66-181DA25598A2}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
@@ -528,7 +525,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="0">A3 +1</f>
+        <f t="shared" ref="A4:A13" si="0">A3 +1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -622,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -640,13 +637,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -664,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -682,53 +679,35 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C14" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>